<commit_message>
new results + evaluation refined
</commit_message>
<xml_diff>
--- a/final samples - final/output.xlsx
+++ b/final samples - final/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH9"/>
+  <dimension ref="A1:CJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,237 +501,377 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_E_EQUAL_LABEL</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_E_EQUAL_SCORE</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_E_WITHIN_LABEL_RANGE</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_T_EQUAL_LABEL</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_T_EQUAL_SCORE</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_T_WITHIN_LABEL_RANGE</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>accuracy_overall_E_SUBSET_OF_GT_EQUAL_LABEL</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_SUBSET_OF_GT_EQUAL_SCORE</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_SUBSET_OF_GT_WITHIN_LABEL_RANGE</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_E_SUBSETEQUAL_OF_GT_EQUAL_LABEL</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_E_SUBSETEQUAL_OF_GT_EQUAL_SCORE</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_E_SUBSETEQUAL_OF_GT_WITHIN_LABEL_RANGE</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_SUBSET_OF_GT_EQUAL_LABEL</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_SUBSET_OF_GT_EQUAL_SCORE</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_SUBSET_OF_GT_WITHIN_LABEL_RANGE</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_T_SUBSETEQUAL_OF_GT_EQUAL_LABEL</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_T_SUBSETEQUAL_OF_GT_EQUAL_SCORE</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_T_SUBSETEQUAL_OF_GT_WITHIN_LABEL_RANGE</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>accuracy_identical_CWE_E</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>accuracy_CWE_GT_SUBSET_OF_E</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>accuracy_CWE_E_SUBSET_OF_GT</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_CWE_GT_SUBSETEQUAL_OF_E</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_CWE_E_SUBSETEQUAL_OF_GT</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>accuracy_identical_CWE_T</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>accuracy_CWE_GT_SUBSET_OF_T</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>accuracy_CWE_T_SUBSET_OF_GT</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_CWE_GT_SUBSETEQUAL_OF_T</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_CWE_T_SUBSETEQUAL_OF_GT</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>accuracy_empty_CWE_E</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>accuracy_empty_CWE_T</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>accuracy_non_overlapped_CWE_E</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>accuracy_non_overlapped_CWE_T</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overlapped_CWE_E</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overlapped_CWE_T</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>accuracy_identical_severity_label</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>accuracy_severity_score_exact_match</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>accuracy_severity_score_label_range</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>accuracy_severity_score_radius_range</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>SEVERITY_ERRORS</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>CWE_ERRORS</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>INVALID_CWE_INFERENCE_counter</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>INVALID_SEVERITY_INFERENCE_counter</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>accuracy_severity_score_radius_range_0.5</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_WITHIN_RADIUS_RANGE_0.5</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_WITHIN_RADIUS_RANGE_0.5</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_GT_SUBSET_OF_E_WITHIN_RADIUS_RANGE_0.5</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_E_WITHIN_RADIUS_RANGE_0.5</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_GT_SUBSET_OF_T_WITHIN_RADIUS_RANGE_0.5</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_T_WITHIN_RADIUS_RANGE_0.5</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_SUBSET_OF_GT_WITHIN_RADIUS_RANGE_0.5</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_E_SUBSETEQUAL_OF_GT_WITHIN_RADIUS_RANGE_0.5</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_SUBSET_OF_GT_WITHIN_RADIUS_RANGE_0.5</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_T_SUBSETEQUAL_OF_GT_WITHIN_RADIUS_RANGE_0.5</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>accuracy_severity_score_radius_range_1</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_WITHIN_RADIUS_RANGE_1</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_WITHIN_RADIUS_RANGE_1</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_GT_SUBSET_OF_E_WITHIN_RADIUS_RANGE_1</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_E_WITHIN_RADIUS_RANGE_1</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_GT_SUBSET_OF_T_WITHIN_RADIUS_RANGE_1</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_T_WITHIN_RADIUS_RANGE_1</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_SUBSET_OF_GT_WITHIN_RADIUS_RANGE_1</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_E_SUBSETEQUAL_OF_GT_WITHIN_RADIUS_RANGE_1</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_SUBSET_OF_GT_WITHIN_RADIUS_RANGE_1</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_T_SUBSETEQUAL_OF_GT_WITHIN_RADIUS_RANGE_1</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>accuracy_severity_score_radius_range_1.5</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_WITHIN_RADIUS_RANGE_1.5</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_WITHIN_RADIUS_RANGE_1.5</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_GT_SUBSET_OF_E_WITHIN_RADIUS_RANGE_1.5</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_E_WITHIN_RADIUS_RANGE_1.5</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_GT_SUBSET_OF_T_WITHIN_RADIUS_RANGE_1.5</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_GT_SUBSETEQUAL_OF_T_WITHIN_RADIUS_RANGE_1.5</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_E_SUBSET_OF_GT_WITHIN_RADIUS_RANGE_1.5</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_E_SUBSETEQUAL_OF_GT_WITHIN_RADIUS_RANGE_1.5</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>accuracy_overall_T_SUBSET_OF_GT_WITHIN_RADIUS_RANGE_1.5</t>
+        </is>
+      </c>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_overall_T_SUBSETEQUAL_OF_GT_WITHIN_RADIUS_RANGE_1.5</t>
         </is>
       </c>
     </row>
@@ -778,145 +918,229 @@
         <v>21.2</v>
       </c>
       <c r="N2" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S2" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="T2" t="n">
         <v>0.6</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>50</v>
-      </c>
       <c r="U2" t="n">
-        <v>8.4</v>
+        <v>0.2</v>
       </c>
       <c r="V2" t="n">
         <v>0.6</v>
       </c>
       <c r="W2" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>50</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>58.4</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="AK2" t="n">
         <v>7.2</v>
       </c>
-      <c r="X2" t="n">
+      <c r="AL2" t="n">
         <v>60.4</v>
       </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="n">
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="AP2" t="n">
         <v>3</v>
       </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="n">
+      <c r="AQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="n">
         <v>31.2</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AS2" t="n">
         <v>24.8</v>
       </c>
-      <c r="AD2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AE2" t="n">
+      <c r="AT2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AU2" t="n">
         <v>1</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AV2" t="n">
         <v>33.4</v>
       </c>
-      <c r="AG2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AH2" t="n">
+      <c r="AW2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AX2" t="n">
         <v>33.4</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AY2" t="n">
         <v>42.8</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AZ2" t="n">
         <v>29</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="BA2" t="n">
         <v>4</v>
       </c>
-      <c r="AL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
+      <c r="BB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="n">
         <v>22.6</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="BE2" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="BF2" t="n">
         <v>1.4</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="BG2" t="n">
         <v>1.8</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="BH2" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="BI2" t="n">
         <v>12.6</v>
       </c>
-      <c r="AS2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU2" t="n">
+      <c r="BJ2" t="n">
+        <v>14</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>9</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="BO2" t="n">
         <v>33.4</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="BP2" t="n">
         <v>14.6</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="BQ2" t="n">
         <v>2.2</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="BR2" t="n">
         <v>3.2</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="BS2" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="BT2" t="n">
         <v>20</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="BU2" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="BV2" t="n">
         <v>0.6</v>
       </c>
-      <c r="BA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="n">
+      <c r="BW2" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="BZ2" t="n">
         <v>42.8</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="CA2" t="n">
         <v>18.4</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="CB2" t="n">
         <v>2.8</v>
       </c>
-      <c r="BE2" t="n">
+      <c r="CC2" t="n">
         <v>4</v>
       </c>
-      <c r="BF2" t="n">
+      <c r="CD2" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="CE2" t="n">
         <v>24.8</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="CF2" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="CG2" t="n">
         <v>0.6</v>
       </c>
-      <c r="BH2" t="n">
-        <v>0</v>
+      <c r="CH2" t="n">
+        <v>19</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="3">
@@ -962,145 +1186,229 @@
         <v>19</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2</v>
+        <v>18</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.2</v>
+        <v>18.4</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.2</v>
+        <v>22.2</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S3" t="n">
-        <v>0.2</v>
+        <v>22.6</v>
       </c>
       <c r="T3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="W3" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AF3" t="n">
         <v>37.8</v>
       </c>
-      <c r="U3" t="n">
+      <c r="AG3" t="n">
         <v>10.2</v>
       </c>
-      <c r="V3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="W3" t="n">
+      <c r="AH3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>48</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>38</v>
+      </c>
+      <c r="AK3" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AL3" t="n">
         <v>48.2</v>
       </c>
-      <c r="Y3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Z3" t="n">
+      <c r="AM3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>57</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AP3" t="n">
         <v>13.2</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AQ3" t="n">
         <v>4.4</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AR3" t="n">
         <v>32.6</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AS3" t="n">
         <v>32.4</v>
       </c>
-      <c r="AD3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AF3" t="n">
+      <c r="AT3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AV3" t="n">
         <v>39.2</v>
       </c>
-      <c r="AG3" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AH3" t="n">
+      <c r="AW3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AX3" t="n">
         <v>39.2</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AY3" t="n">
         <v>48.4</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AZ3" t="n">
         <v>23</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="BA3" t="n">
         <v>14</v>
       </c>
-      <c r="AL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
+      <c r="BB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="n">
         <v>21.4</v>
       </c>
-      <c r="AO3" t="n">
+      <c r="BE3" t="n">
         <v>7.4</v>
       </c>
-      <c r="AP3" t="n">
+      <c r="BF3" t="n">
         <v>3</v>
       </c>
-      <c r="AQ3" t="n">
+      <c r="BG3" t="n">
         <v>2.6</v>
       </c>
-      <c r="AR3" t="n">
+      <c r="BH3" t="n">
+        <v>10</v>
+      </c>
+      <c r="BI3" t="n">
         <v>9.199999999999999</v>
       </c>
-      <c r="AS3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU3" t="n">
+      <c r="BJ3" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>3</v>
+      </c>
+      <c r="BO3" t="n">
         <v>34.4</v>
       </c>
-      <c r="AV3" t="n">
+      <c r="BP3" t="n">
         <v>12.8</v>
       </c>
-      <c r="AW3" t="n">
+      <c r="BQ3" t="n">
         <v>3.6</v>
       </c>
-      <c r="AX3" t="n">
+      <c r="BR3" t="n">
         <v>3.8</v>
       </c>
-      <c r="AY3" t="n">
+      <c r="BS3" t="n">
         <v>16.6</v>
       </c>
-      <c r="AZ3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BB3" t="n">
+      <c r="BT3" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>13</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="BZ3" t="n">
         <v>48.4</v>
       </c>
-      <c r="BC3" t="n">
+      <c r="CA3" t="n">
         <v>18.4</v>
       </c>
-      <c r="BD3" t="n">
+      <c r="CB3" t="n">
         <v>4.6</v>
       </c>
-      <c r="BE3" t="n">
+      <c r="CC3" t="n">
         <v>5.2</v>
       </c>
-      <c r="BF3" t="n">
+      <c r="CD3" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="CE3" t="n">
         <v>24.2</v>
       </c>
-      <c r="BG3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>0.2</v>
+      <c r="CF3" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>4.8</v>
       </c>
     </row>
     <row r="4">
@@ -1146,145 +1454,229 @@
         <v>18.4</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2</v>
+        <v>14.6</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2</v>
+        <v>14.6</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>20.4</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>19.8</v>
       </c>
       <c r="T4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="W4" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AF4" t="n">
         <v>42.6</v>
       </c>
-      <c r="U4" t="n">
+      <c r="AG4" t="n">
         <v>6.4</v>
       </c>
-      <c r="V4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="W4" t="n">
+      <c r="AH4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>49</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="AK4" t="n">
         <v>4</v>
       </c>
-      <c r="X4" t="n">
+      <c r="AL4" t="n">
         <v>57.6</v>
       </c>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="n">
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>61.6</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP4" t="n">
         <v>14.2</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AQ4" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AR4" t="n">
         <v>32.6</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AS4" t="n">
         <v>26.2</v>
       </c>
-      <c r="AD4" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AF4" t="n">
+      <c r="AT4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AV4" t="n">
         <v>34.2</v>
       </c>
-      <c r="AG4" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AH4" t="n">
+      <c r="AW4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AX4" t="n">
         <v>33</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AY4" t="n">
         <v>42.4</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AZ4" t="n">
         <v>15</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="BA4" t="n">
         <v>17</v>
       </c>
-      <c r="AL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="n">
+      <c r="BB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD4" t="n">
         <v>21</v>
       </c>
-      <c r="AO4" t="n">
+      <c r="BE4" t="n">
         <v>7</v>
       </c>
-      <c r="AP4" t="n">
+      <c r="BF4" t="n">
         <v>1.2</v>
       </c>
-      <c r="AQ4" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AR4" t="n">
+      <c r="BG4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="BI4" t="n">
         <v>9.6</v>
       </c>
-      <c r="AS4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AT4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU4" t="n">
+      <c r="BJ4" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="BO4" t="n">
         <v>32</v>
       </c>
-      <c r="AV4" t="n">
+      <c r="BP4" t="n">
         <v>12</v>
       </c>
-      <c r="AW4" t="n">
+      <c r="BQ4" t="n">
         <v>1.6</v>
       </c>
-      <c r="AX4" t="n">
+      <c r="BR4" t="n">
         <v>1.6</v>
       </c>
-      <c r="AY4" t="n">
+      <c r="BS4" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="BT4" t="n">
         <v>17</v>
       </c>
-      <c r="AZ4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB4" t="n">
+      <c r="BU4" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="BZ4" t="n">
         <v>42.4</v>
       </c>
-      <c r="BC4" t="n">
+      <c r="CA4" t="n">
         <v>16.4</v>
       </c>
-      <c r="BD4" t="n">
+      <c r="CB4" t="n">
         <v>2.2</v>
       </c>
-      <c r="BE4" t="n">
+      <c r="CC4" t="n">
         <v>2.2</v>
       </c>
-      <c r="BF4" t="n">
+      <c r="CD4" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="CE4" t="n">
         <v>23</v>
       </c>
-      <c r="BG4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>0</v>
+      <c r="CF4" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>2.2</v>
       </c>
     </row>
     <row r="5">
@@ -1330,145 +1722,229 @@
         <v>23.4</v>
       </c>
       <c r="N5" t="n">
+        <v>17</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S5" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="T5" t="n">
         <v>0.8</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="T5" t="n">
-        <v>49.8</v>
-      </c>
       <c r="U5" t="n">
-        <v>5.4</v>
+        <v>0.2</v>
       </c>
       <c r="V5" t="n">
         <v>0.8</v>
       </c>
       <c r="W5" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>55.2</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>50.59999999999999</v>
+      </c>
+      <c r="AK5" t="n">
         <v>2.8</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AL5" t="n">
         <v>67.2</v>
       </c>
-      <c r="Y5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Z5" t="n">
+      <c r="AM5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>70</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP5" t="n">
         <v>5</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AQ5" t="n">
         <v>0.6</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AR5" t="n">
         <v>38.2</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AS5" t="n">
         <v>27.6</v>
       </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="n">
         <v>0.8</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AV5" t="n">
         <v>37.6</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AW5" t="n">
         <v>0.6</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AX5" t="n">
         <v>37.4</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AY5" t="n">
         <v>48.6</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AZ5" t="n">
         <v>4</v>
       </c>
-      <c r="AK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
+      <c r="BA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD5" t="n">
         <v>24.2</v>
       </c>
-      <c r="AO5" t="n">
+      <c r="BE5" t="n">
         <v>9.4</v>
       </c>
-      <c r="AP5" t="n">
+      <c r="BF5" t="n">
         <v>0.6</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="BG5" t="n">
         <v>1.2</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="BH5" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="BI5" t="n">
         <v>14.8</v>
       </c>
-      <c r="AS5" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU5" t="n">
+      <c r="BJ5" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="BO5" t="n">
         <v>35.8</v>
       </c>
-      <c r="AV5" t="n">
+      <c r="BP5" t="n">
         <v>14.4</v>
       </c>
-      <c r="AW5" t="n">
+      <c r="BQ5" t="n">
         <v>1</v>
       </c>
-      <c r="AX5" t="n">
+      <c r="BR5" t="n">
         <v>1.8</v>
       </c>
-      <c r="AY5" t="n">
+      <c r="BS5" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="BT5" t="n">
         <v>22.4</v>
       </c>
-      <c r="AZ5" t="n">
+      <c r="BU5" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="BV5" t="n">
         <v>0.6</v>
       </c>
-      <c r="BA5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BB5" t="n">
+      <c r="BW5" t="n">
+        <v>15</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="BZ5" t="n">
         <v>48.6</v>
       </c>
-      <c r="BC5" t="n">
+      <c r="CA5" t="n">
         <v>21.4</v>
       </c>
-      <c r="BD5" t="n">
+      <c r="CB5" t="n">
         <v>1.6</v>
       </c>
-      <c r="BE5" t="n">
+      <c r="CC5" t="n">
         <v>2</v>
       </c>
-      <c r="BF5" t="n">
+      <c r="CD5" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="CE5" t="n">
         <v>29.6</v>
       </c>
-      <c r="BG5" t="n">
+      <c r="CF5" t="n">
+        <v>31.2</v>
+      </c>
+      <c r="CG5" t="n">
         <v>0.6</v>
       </c>
-      <c r="BH5" t="n">
-        <v>0.2</v>
+      <c r="CH5" t="n">
+        <v>22</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="6">
@@ -1514,145 +1990,229 @@
         <v>0.6</v>
       </c>
       <c r="N6" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="T6" t="n">
         <v>0.6</v>
       </c>
-      <c r="O6" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="T6" t="n">
-        <v>68</v>
-      </c>
       <c r="U6" t="n">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="V6" t="n">
         <v>0.6</v>
       </c>
       <c r="W6" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="AF6" t="n">
         <v>68</v>
       </c>
-      <c r="X6" t="n">
+      <c r="AG6" t="n">
         <v>1.2</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AH6" t="n">
         <v>0.6</v>
       </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
+      <c r="AI6" t="n">
+        <v>69.2</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>68</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>69.2</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR6" t="n">
         <v>30.2</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AS6" t="n">
         <v>30.2</v>
       </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="n">
+      <c r="AT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="n">
         <v>60.2</v>
       </c>
-      <c r="AG6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AH6" t="n">
+      <c r="AW6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AX6" t="n">
         <v>59.6</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AY6" t="n">
         <v>71.2</v>
       </c>
-      <c r="AJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="n">
+      <c r="AZ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD6" t="n">
         <v>39.4</v>
       </c>
-      <c r="AO6" t="n">
+      <c r="BE6" t="n">
         <v>29.2</v>
       </c>
-      <c r="AP6" t="n">
+      <c r="BF6" t="n">
         <v>29.2</v>
       </c>
-      <c r="AQ6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AT6" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AU6" t="n">
+      <c r="BG6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="BO6" t="n">
         <v>56.6</v>
       </c>
-      <c r="AV6" t="n">
+      <c r="BP6" t="n">
         <v>41</v>
       </c>
-      <c r="AW6" t="n">
+      <c r="BQ6" t="n">
         <v>41</v>
       </c>
-      <c r="AX6" t="n">
+      <c r="BR6" t="n">
         <v>0.8</v>
       </c>
-      <c r="AY6" t="n">
+      <c r="BS6" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="BT6" t="n">
         <v>0.8</v>
       </c>
-      <c r="AZ6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BB6" t="n">
+      <c r="BU6" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="BV6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BW6" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="BX6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="BZ6" t="n">
         <v>71.2</v>
       </c>
-      <c r="BC6" t="n">
+      <c r="CA6" t="n">
         <v>51.2</v>
       </c>
-      <c r="BD6" t="n">
+      <c r="CB6" t="n">
         <v>51.2</v>
       </c>
-      <c r="BE6" t="n">
+      <c r="CC6" t="n">
         <v>0.8</v>
       </c>
-      <c r="BF6" t="n">
+      <c r="CD6" t="n">
+        <v>52</v>
+      </c>
+      <c r="CE6" t="n">
         <v>0.8</v>
       </c>
-      <c r="BG6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>0.4</v>
+      <c r="CF6" t="n">
+        <v>52</v>
+      </c>
+      <c r="CG6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="CI6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="CJ6" t="n">
+        <v>51.6</v>
       </c>
     </row>
     <row r="7">
@@ -1698,145 +2258,229 @@
         <v>0.4</v>
       </c>
       <c r="N7" t="n">
-        <v>0.4</v>
+        <v>45.6</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>0.4</v>
+        <v>45.6</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.4</v>
+        <v>45.6</v>
       </c>
       <c r="R7" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0.4</v>
+        <v>45.6</v>
       </c>
       <c r="T7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W7" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="AF7" t="n">
         <v>63.6</v>
       </c>
-      <c r="U7" t="n">
+      <c r="AG7" t="n">
         <v>1</v>
       </c>
-      <c r="V7" t="n">
+      <c r="AH7" t="n">
         <v>0.6</v>
       </c>
-      <c r="W7" t="n">
+      <c r="AI7" t="n">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>64.2</v>
+      </c>
+      <c r="AK7" t="n">
         <v>63.6</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AL7" t="n">
         <v>1</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AM7" t="n">
         <v>0.6</v>
       </c>
-      <c r="Z7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB7" t="n">
+      <c r="AN7" t="n">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>64.2</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="n">
         <v>31.6</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AS7" t="n">
         <v>31.6</v>
       </c>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="n">
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="n">
         <v>61.2</v>
       </c>
-      <c r="AG7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AH7" t="n">
+      <c r="AW7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AX7" t="n">
         <v>60.8</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AY7" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AZ7" t="n">
         <v>16</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="BA7" t="n">
         <v>6</v>
       </c>
-      <c r="AL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="n">
+      <c r="BB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD7" t="n">
         <v>39</v>
       </c>
-      <c r="AO7" t="n">
+      <c r="BE7" t="n">
         <v>26.8</v>
       </c>
-      <c r="AP7" t="n">
+      <c r="BF7" t="n">
         <v>26.8</v>
       </c>
-      <c r="AQ7" t="n">
+      <c r="BG7" t="n">
         <v>0.6</v>
       </c>
-      <c r="AR7" t="n">
+      <c r="BH7" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="BI7" t="n">
         <v>0.6</v>
       </c>
-      <c r="AS7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AT7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AU7" t="n">
+      <c r="BJ7" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>27</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>27</v>
+      </c>
+      <c r="BO7" t="n">
         <v>59.4</v>
       </c>
-      <c r="AV7" t="n">
+      <c r="BP7" t="n">
         <v>42</v>
       </c>
-      <c r="AW7" t="n">
+      <c r="BQ7" t="n">
         <v>42</v>
       </c>
-      <c r="AX7" t="n">
+      <c r="BR7" t="n">
         <v>0.8</v>
       </c>
-      <c r="AY7" t="n">
+      <c r="BS7" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="BT7" t="n">
         <v>0.8</v>
       </c>
-      <c r="AZ7" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BA7" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BB7" t="n">
+      <c r="BU7" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="BV7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BW7" t="n">
+        <v>42.4</v>
+      </c>
+      <c r="BX7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>42.4</v>
+      </c>
+      <c r="BZ7" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="BC7" t="n">
+      <c r="CA7" t="n">
         <v>50.6</v>
       </c>
-      <c r="BD7" t="n">
+      <c r="CB7" t="n">
         <v>50.6</v>
       </c>
-      <c r="BE7" t="n">
+      <c r="CC7" t="n">
         <v>0.8</v>
       </c>
-      <c r="BF7" t="n">
+      <c r="CD7" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="CE7" t="n">
         <v>0.8</v>
       </c>
-      <c r="BG7" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>0.4</v>
+      <c r="CF7" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="CG7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>51</v>
+      </c>
+      <c r="CI7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="CJ7" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="8">
@@ -1882,145 +2526,229 @@
         <v>1.4</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2</v>
+        <v>43.2</v>
       </c>
       <c r="O8" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2</v>
+        <v>43</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2</v>
+        <v>43.2</v>
       </c>
       <c r="R8" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0.2</v>
+        <v>43</v>
       </c>
       <c r="T8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="W8" t="n">
+        <v>42</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>42</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="AF8" t="n">
         <v>62.8</v>
       </c>
-      <c r="U8" t="n">
+      <c r="AG8" t="n">
         <v>2.4</v>
       </c>
-      <c r="V8" t="n">
+      <c r="AH8" t="n">
         <v>0.8</v>
       </c>
-      <c r="W8" t="n">
+      <c r="AI8" t="n">
+        <v>65.2</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>63.59999999999999</v>
+      </c>
+      <c r="AK8" t="n">
         <v>62.8</v>
       </c>
-      <c r="X8" t="n">
+      <c r="AL8" t="n">
         <v>2.4</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="AM8" t="n">
         <v>0.8</v>
       </c>
-      <c r="Z8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" t="n">
+      <c r="AN8" t="n">
+        <v>65.2</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>63.59999999999999</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR8" t="n">
         <v>31.2</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AS8" t="n">
         <v>31.2</v>
       </c>
-      <c r="AD8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" t="n">
+      <c r="AT8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="n">
         <v>57.8</v>
       </c>
-      <c r="AG8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AH8" t="n">
+      <c r="AW8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AX8" t="n">
         <v>57.4</v>
       </c>
-      <c r="AI8" t="n">
+      <c r="AY8" t="n">
         <v>71</v>
       </c>
-      <c r="AJ8" t="n">
+      <c r="AZ8" t="n">
         <v>14</v>
       </c>
-      <c r="AK8" t="n">
+      <c r="BA8" t="n">
         <v>14</v>
       </c>
-      <c r="AL8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN8" t="n">
+      <c r="BB8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD8" t="n">
         <v>37.2</v>
       </c>
-      <c r="AO8" t="n">
+      <c r="BE8" t="n">
         <v>25.2</v>
       </c>
-      <c r="AP8" t="n">
+      <c r="BF8" t="n">
         <v>25.2</v>
       </c>
-      <c r="AQ8" t="n">
+      <c r="BG8" t="n">
         <v>1</v>
       </c>
-      <c r="AR8" t="n">
+      <c r="BH8" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="BI8" t="n">
         <v>1</v>
       </c>
-      <c r="AS8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AT8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AU8" t="n">
+      <c r="BJ8" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="BO8" t="n">
         <v>54.8</v>
       </c>
-      <c r="AV8" t="n">
+      <c r="BP8" t="n">
         <v>37.4</v>
       </c>
-      <c r="AW8" t="n">
+      <c r="BQ8" t="n">
         <v>37.4</v>
       </c>
-      <c r="AX8" t="n">
+      <c r="BR8" t="n">
         <v>1.6</v>
       </c>
-      <c r="AY8" t="n">
+      <c r="BS8" t="n">
+        <v>39</v>
+      </c>
+      <c r="BT8" t="n">
         <v>1.6</v>
       </c>
-      <c r="AZ8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BA8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BB8" t="n">
+      <c r="BU8" t="n">
+        <v>39</v>
+      </c>
+      <c r="BV8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BW8" t="n">
+        <v>37.8</v>
+      </c>
+      <c r="BX8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BY8" t="n">
+        <v>37.8</v>
+      </c>
+      <c r="BZ8" t="n">
         <v>71</v>
       </c>
-      <c r="BC8" t="n">
+      <c r="CA8" t="n">
         <v>47.8</v>
       </c>
-      <c r="BD8" t="n">
+      <c r="CB8" t="n">
         <v>47.8</v>
       </c>
-      <c r="BE8" t="n">
+      <c r="CC8" t="n">
         <v>1.8</v>
       </c>
-      <c r="BF8" t="n">
+      <c r="CD8" t="n">
+        <v>49.59999999999999</v>
+      </c>
+      <c r="CE8" t="n">
         <v>1.8</v>
       </c>
-      <c r="BG8" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="BH8" t="n">
-        <v>0.4</v>
+      <c r="CF8" t="n">
+        <v>49.59999999999999</v>
+      </c>
+      <c r="CG8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="CH8" t="n">
+        <v>48.2</v>
+      </c>
+      <c r="CI8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="CJ8" t="n">
+        <v>48.2</v>
       </c>
     </row>
     <row r="9">
@@ -2066,145 +2794,229 @@
         <v>0.8</v>
       </c>
       <c r="N9" t="n">
-        <v>0.4</v>
+        <v>45.4</v>
       </c>
       <c r="O9" t="n">
         <v>0.2</v>
       </c>
       <c r="P9" t="n">
-        <v>0.4</v>
+        <v>45.2</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.4</v>
+        <v>45.4</v>
       </c>
       <c r="R9" t="n">
         <v>0.2</v>
       </c>
       <c r="S9" t="n">
-        <v>0.4</v>
+        <v>45.2</v>
       </c>
       <c r="T9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W9" t="n">
+        <v>45</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>45</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="AF9" t="n">
         <v>65</v>
       </c>
-      <c r="U9" t="n">
+      <c r="AG9" t="n">
         <v>1.4</v>
       </c>
-      <c r="V9" t="n">
+      <c r="AH9" t="n">
         <v>0.8</v>
       </c>
-      <c r="W9" t="n">
+      <c r="AI9" t="n">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="AK9" t="n">
         <v>65</v>
       </c>
-      <c r="X9" t="n">
+      <c r="AL9" t="n">
         <v>1.4</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AM9" t="n">
         <v>0.8</v>
       </c>
-      <c r="Z9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB9" t="n">
+      <c r="AN9" t="n">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" t="n">
         <v>32.8</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AS9" t="n">
         <v>32.8</v>
       </c>
-      <c r="AD9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" t="n">
+      <c r="AT9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="n">
         <v>61.2</v>
       </c>
-      <c r="AG9" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AH9" t="n">
+      <c r="AW9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AX9" t="n">
         <v>61</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AY9" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="AJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="n">
+      <c r="AZ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD9" t="n">
         <v>39.4</v>
       </c>
-      <c r="AO9" t="n">
+      <c r="BE9" t="n">
         <v>27</v>
       </c>
-      <c r="AP9" t="n">
+      <c r="BF9" t="n">
         <v>27</v>
       </c>
-      <c r="AQ9" t="n">
+      <c r="BG9" t="n">
         <v>0.8</v>
       </c>
-      <c r="AR9" t="n">
+      <c r="BH9" t="n">
+        <v>27.8</v>
+      </c>
+      <c r="BI9" t="n">
         <v>0.8</v>
       </c>
-      <c r="AS9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AT9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AU9" t="n">
+      <c r="BJ9" t="n">
+        <v>27.8</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>27.2</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>27.2</v>
+      </c>
+      <c r="BO9" t="n">
         <v>58</v>
       </c>
-      <c r="AV9" t="n">
+      <c r="BP9" t="n">
         <v>39.8</v>
       </c>
-      <c r="AW9" t="n">
+      <c r="BQ9" t="n">
         <v>39.8</v>
       </c>
-      <c r="AX9" t="n">
+      <c r="BR9" t="n">
         <v>1.2</v>
       </c>
-      <c r="AY9" t="n">
+      <c r="BS9" t="n">
+        <v>41</v>
+      </c>
+      <c r="BT9" t="n">
         <v>1.2</v>
       </c>
-      <c r="AZ9" t="n">
+      <c r="BU9" t="n">
+        <v>41</v>
+      </c>
+      <c r="BV9" t="n">
         <v>0.6</v>
       </c>
-      <c r="BA9" t="n">
+      <c r="BW9" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="BX9" t="n">
         <v>0.6</v>
       </c>
-      <c r="BB9" t="n">
+      <c r="BY9" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="BZ9" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="BC9" t="n">
+      <c r="CA9" t="n">
         <v>49.8</v>
       </c>
-      <c r="BD9" t="n">
+      <c r="CB9" t="n">
         <v>49.8</v>
       </c>
-      <c r="BE9" t="n">
+      <c r="CC9" t="n">
         <v>1.2</v>
       </c>
-      <c r="BF9" t="n">
+      <c r="CD9" t="n">
+        <v>51</v>
+      </c>
+      <c r="CE9" t="n">
         <v>1.2</v>
       </c>
-      <c r="BG9" t="n">
+      <c r="CF9" t="n">
+        <v>51</v>
+      </c>
+      <c r="CG9" t="n">
         <v>0.6</v>
       </c>
-      <c r="BH9" t="n">
+      <c r="CH9" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="CI9" t="n">
         <v>0.6</v>
+      </c>
+      <c r="CJ9" t="n">
+        <v>50.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
erorrs and invalids measured in percentage
</commit_message>
<xml_diff>
--- a/final samples - final/output.xlsx
+++ b/final samples - final/output.xlsx
@@ -691,22 +691,22 @@
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>SEVERITY_ERRORS</t>
+          <t>accuracy_SEVERITY_ERRORS</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>CWE_ERRORS</t>
+          <t>accuracy_CWE_ERRORS</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>INVALID_CWE_INFERENCE_counter</t>
+          <t>accuracy_INVALID_CWE_INFERENCE_counter</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>INVALID_SEVERITY_INFERENCE_counter</t>
+          <t>accuracy_INVALID_SEVERITY_INFERENCE_counter</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
@@ -1032,10 +1032,10 @@
         <v>42.8</v>
       </c>
       <c r="AZ2" t="n">
-        <v>29</v>
+        <v>5.8</v>
       </c>
       <c r="BA2" t="n">
-        <v>4</v>
+        <v>0.8</v>
       </c>
       <c r="BB2" t="n">
         <v>0</v>
@@ -1300,10 +1300,10 @@
         <v>48.4</v>
       </c>
       <c r="AZ3" t="n">
-        <v>23</v>
+        <v>4.6</v>
       </c>
       <c r="BA3" t="n">
-        <v>14</v>
+        <v>2.8</v>
       </c>
       <c r="BB3" t="n">
         <v>0</v>
@@ -1568,10 +1568,10 @@
         <v>42.4</v>
       </c>
       <c r="AZ4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="BA4" t="n">
-        <v>17</v>
+        <v>3.4</v>
       </c>
       <c r="BB4" t="n">
         <v>0</v>
@@ -1836,7 +1836,7 @@
         <v>48.6</v>
       </c>
       <c r="AZ5" t="n">
-        <v>4</v>
+        <v>0.8</v>
       </c>
       <c r="BA5" t="n">
         <v>0</v>
@@ -2372,10 +2372,10 @@
         <v>73.59999999999999</v>
       </c>
       <c r="AZ7" t="n">
-        <v>16</v>
+        <v>3.2</v>
       </c>
       <c r="BA7" t="n">
-        <v>6</v>
+        <v>1.2</v>
       </c>
       <c r="BB7" t="n">
         <v>0</v>
@@ -2640,10 +2640,10 @@
         <v>71</v>
       </c>
       <c r="AZ8" t="n">
-        <v>14</v>
+        <v>2.8</v>
       </c>
       <c r="BA8" t="n">
-        <v>14</v>
+        <v>2.8</v>
       </c>
       <c r="BB8" t="n">
         <v>0</v>

</xml_diff>